<commit_message>
first structuring of python code, added also first unit tests
</commit_message>
<xml_diff>
--- a/mgt/Tasks.xlsx
+++ b/mgt/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2B6303-058F-4FAF-844B-9FD63B0E844C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC6C06C-A37B-41A7-AD43-3C41D9504FFF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Python Tutorial/Course</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Status Date</t>
   </si>
   <si>
-    <t>Comments were created to explain the Random Walk process, coefficients and reasoning. For now however the noise component was removed from RBD, noise to be included in the dynamic model ( forces and torques).</t>
-  </si>
-  <si>
     <t>Create Quad model/class for forces and torques</t>
   </si>
   <si>
@@ -76,7 +73,13 @@
     <t>https://docs.python-guide.org/writing/structure/</t>
   </si>
   <si>
-    <t>Reading</t>
+    <t>Comments were created to explain the Random Walk process, coefficients and reasoning. For now however the noise component was removed from RBD, noise to be included in the dynamic model (forces and torques).</t>
+  </si>
+  <si>
+    <t>Done Reading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ongoing </t>
   </si>
 </sst>
 </file>
@@ -418,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -431,6 +434,7 @@
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="26.44140625" customWidth="1"/>
     <col min="5" max="5" width="11.77734375" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
     <col min="7" max="7" width="83.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -470,82 +474,89 @@
         <v>43635</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
         <v>18</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="C5" s="2"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C6" s="2">
         <v>43634</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C6" s="2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C7" s="2">
         <v>43635</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>3</v>
-      </c>
-      <c r="C7" s="2">
-        <v>43634</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="C8" s="2">
         <v>43634</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2">
+        <v>43634</v>
+      </c>
+      <c r="E9" s="2">
         <v>43635</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="C10" s="2">
         <v>43635</v>
       </c>
     </row>

</xml_diff>

<commit_message>
worked on test cases for the rigid body class
</commit_message>
<xml_diff>
--- a/mgt/Tasks.xlsx
+++ b/mgt/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC6C06C-A37B-41A7-AD43-3C41D9504FFF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1891093F-91B3-45E5-878B-A544789E17AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Python Tutorial/Course</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Create Quad model/class for forces and torques</t>
   </si>
   <si>
-    <t>Find topics</t>
-  </si>
-  <si>
     <t xml:space="preserve">Topic 1: How to structure code </t>
   </si>
   <si>
@@ -76,10 +73,28 @@
     <t>Comments were created to explain the Random Walk process, coefficients and reasoning. For now however the noise component was removed from RBD, noise to be included in the dynamic model (forces and torques).</t>
   </si>
   <si>
-    <t>Done Reading</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ongoing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enlarge the utils library with Rotation - Euler Angles transformation to be able to do plotting in the test cases </t>
+  </si>
+  <si>
+    <t>doc strings: https://www.python.org/dev/peps/pep-0257/</t>
+  </si>
+  <si>
+    <t>style guide for python code: https://www.python.org/dev/peps/pep-0008/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improve the logger , and write to files </t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>ToDo</t>
+  </si>
+  <si>
+    <t>Find topics, read documents</t>
   </si>
 </sst>
 </file>
@@ -421,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,97 +489,141 @@
         <v>43635</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
-      <c r="G5" s="4"/>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="C6" s="2"/>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C7" s="2">
         <v>43634</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C7" s="2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C8" s="2">
         <v>43635</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>3</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>3</v>
-      </c>
-      <c r="C8" s="2">
-        <v>43634</v>
-      </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="C9" s="2">
         <v>43634</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2">
+        <v>43634</v>
+      </c>
+      <c r="E10" s="2">
         <v>43635</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="G10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>5</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C11" s="2">
+        <v>43635</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="2">
+        <v>43635</v>
+      </c>
+      <c r="E12" s="2">
+        <v>43635</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="2">
         <v>43635</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1" xr:uid="{9F407E9B-9C8D-4E2F-929C-8FDE3A9211C3}"/>
+    <hyperlink ref="G5" r:id="rId2" display="https://www.python.org/dev/peps/pep-0008/" xr:uid="{2115ECD9-1B72-4573-A8FF-B47D4F0E7727}"/>
+    <hyperlink ref="G6" r:id="rId3" display="https://www.python.org/dev/peps/pep-0257/" xr:uid="{A47415FF-60E2-4A53-89B4-48CD862F7193}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
logger, testcases, rigid body with quaternions
</commit_message>
<xml_diff>
--- a/mgt/Tasks.xlsx
+++ b/mgt/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5500E9CF-8B9F-4415-9412-A5912149BBD0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0394ADE6-1486-43FD-B888-6E6D1C7CC486}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>Python Tutorial/Course</t>
   </si>
@@ -116,6 +116,24 @@
   </si>
   <si>
     <t>Add quaternions function and compare results with rotation matrix</t>
+  </si>
+  <si>
+    <t>find a tool to extarct documentation from the docstrings to test it works ok</t>
+  </si>
+  <si>
+    <t>use python help() function, as described here https://wiki.python.org/moin/DocumentationTools</t>
+  </si>
+  <si>
+    <t>Topic 3: NumPy tutorial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">have timing left </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> to investigate more numerically stable formulas, see if I can do better in tests</t>
+  </si>
+  <si>
+    <t>enough for this time, open new issue again if needed</t>
   </si>
 </sst>
 </file>
@@ -457,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -609,120 +627,155 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="2"/>
-      <c r="D13" s="1"/>
+      <c r="C13" s="2">
+        <v>43636</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="C14" s="2"/>
+      <c r="D14" s="1"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>2</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C15" s="2">
         <v>43634</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C15" s="2">
-        <v>43635</v>
-      </c>
-      <c r="D15" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C16" s="2">
+        <v>43635</v>
+      </c>
+      <c r="D16" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>3</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>3</v>
-      </c>
-      <c r="C16" s="2">
-        <v>43634</v>
-      </c>
-      <c r="F16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>4</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="C17" s="2">
         <v>43634</v>
       </c>
-      <c r="E17" s="2">
-        <v>43635</v>
-      </c>
       <c r="F17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="2">
+        <v>43634</v>
+      </c>
+      <c r="E18" s="2">
+        <v>43635</v>
+      </c>
+      <c r="F18" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>5</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="2">
-        <v>43635</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="C19" s="2">
+        <v>43635</v>
+      </c>
+      <c r="F19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19">
+    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>6</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="2">
-        <v>43635</v>
-      </c>
-      <c r="E19" s="2">
-        <v>43635</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="C20" s="2">
+        <v>43635</v>
+      </c>
+      <c r="E20" s="2">
+        <v>43635</v>
+      </c>
+      <c r="F20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>7</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="2">
-        <v>43635</v>
-      </c>
-      <c r="F20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="C21" s="2">
+        <v>43635</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>8</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="2">
-        <v>43635</v>
-      </c>
-      <c r="F21" t="s">
-        <v>22</v>
+      <c r="C22" s="2">
+        <v>43635</v>
+      </c>
+      <c r="F22" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>9</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="2">
+        <v>43636</v>
+      </c>
+      <c r="F23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more updates to the ftau model
</commit_message>
<xml_diff>
--- a/mgt/Tasks.xlsx
+++ b/mgt/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201C90D0-C193-4268-85EB-F16A615303C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B0E65D-9E4E-4749-BB2D-C21E059597BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Python Tutorial/Course</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>enough for this time, open new issue again if needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read all again about first order systems </t>
   </si>
 </sst>
 </file>
@@ -469,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -663,6 +666,9 @@
       <c r="C17" s="2">
         <v>43634</v>
       </c>
+      <c r="E17" s="2">
+        <v>43636</v>
+      </c>
       <c r="F17" t="s">
         <v>20</v>
       </c>
@@ -745,6 +751,9 @@
       <c r="C22" s="2">
         <v>43635</v>
       </c>
+      <c r="E22" s="2">
+        <v>43636</v>
+      </c>
       <c r="F22" t="s">
         <v>20</v>
       </c>
@@ -762,11 +771,25 @@
       <c r="C23" s="2">
         <v>43636</v>
       </c>
+      <c r="E23" s="2">
+        <v>43636</v>
+      </c>
       <c r="F23" t="s">
         <v>20</v>
       </c>
       <c r="G23" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="2">
+        <v>43637</v>
+      </c>
+      <c r="F24" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to ftau model
</commit_message>
<xml_diff>
--- a/mgt/Tasks.xlsx
+++ b/mgt/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14A0AD5-FA85-43B7-9254-F60D531614F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E8A579-99F5-4941-938F-CE47005E26EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>Python Tutorial/Course</t>
   </si>
   <si>
-    <t>Find One</t>
-  </si>
-  <si>
     <t>Matplotlib Tutorial/Course</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
     <t>Status Date</t>
   </si>
   <si>
-    <t>Create Quad model/class for forces and torques</t>
-  </si>
-  <si>
     <t>Ongoing</t>
   </si>
   <si>
@@ -67,9 +61,6 @@
     <t>Comments were created to explain the Random Walk process, coefficients and reasoning. For now however the noise component was removed from RBD, noise to be included in the dynamic model (forces and torques).</t>
   </si>
   <si>
-    <t xml:space="preserve">Ongoing </t>
-  </si>
-  <si>
     <t xml:space="preserve">Enlarge the utils library with Rotation - Euler Angles transformation to be able to do plotting in the test cases </t>
   </si>
   <si>
@@ -134,6 +125,12 @@
   </si>
   <si>
     <t xml:space="preserve">almost done, consider adding a motor FOS step response, and to add configurable noise </t>
+  </si>
+  <si>
+    <t>https://realpython.com/python-matplotlib-guide/#reader-comments</t>
+  </si>
+  <si>
+    <t>Create Quad model for forces and torques</t>
   </si>
 </sst>
 </file>
@@ -475,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -494,22 +491,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -528,52 +525,52 @@
         <v>43635</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E4" s="2">
         <v>43635</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C7" s="2"/>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -582,10 +579,10 @@
         <v>43635</v>
       </c>
       <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -594,10 +591,10 @@
         <v>43635</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -605,10 +602,10 @@
         <v>43635</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -616,14 +613,14 @@
       <c r="C11" s="2"/>
       <c r="D11" s="1"/>
       <c r="G11" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C12" s="2"/>
       <c r="D12" s="1"/>
       <c r="G12" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -631,7 +628,7 @@
         <v>43636</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G13" s="4"/>
     </row>
@@ -645,160 +642,164 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2">
         <v>43634</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C16" s="2">
-        <v>43635</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1</v>
+        <v>43638</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="C17" s="2"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>3</v>
       </c>
-      <c r="B17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="2">
-        <v>43634</v>
-      </c>
-      <c r="E17" s="2">
-        <v>43636</v>
-      </c>
-      <c r="F17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>4</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>4</v>
+      <c r="B18" t="s">
+        <v>2</v>
       </c>
       <c r="C18" s="2">
         <v>43634</v>
       </c>
       <c r="E18" s="2">
-        <v>43635</v>
+        <v>43636</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="2">
+        <v>43634</v>
+      </c>
+      <c r="E19" s="2">
+        <v>43635</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>5</v>
       </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="2">
-        <v>43635</v>
-      </c>
-      <c r="F19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="2">
+        <v>43635</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>6</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="2">
+        <v>43635</v>
+      </c>
+      <c r="E21" s="2">
+        <v>43635</v>
+      </c>
+      <c r="F21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="2">
-        <v>43635</v>
-      </c>
-      <c r="E20" s="2">
-        <v>43635</v>
-      </c>
-      <c r="F20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>7</v>
-      </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="2">
-        <v>43635</v>
-      </c>
-      <c r="F21" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>8</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="C22" s="2">
         <v>43635</v>
       </c>
-      <c r="E22" s="2">
-        <v>43636</v>
-      </c>
       <c r="F22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C23" s="2">
-        <v>43636</v>
+        <v>43635</v>
       </c>
       <c r="E23" s="2">
         <v>43636</v>
       </c>
       <c r="F23" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>9</v>
+      </c>
       <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C24" s="2">
+        <v>43636</v>
+      </c>
+      <c r="E24" s="2">
+        <v>43636</v>
+      </c>
+      <c r="F24" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="2">
         <v>43637</v>
       </c>
-      <c r="F24" t="s">
-        <v>21</v>
+      <c r="F25" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -811,8 +812,9 @@
     <hyperlink ref="G7" r:id="rId6" location="why-we-need-pep-8" xr:uid="{BABF3B79-FEBC-4757-A901-5F528B5760A1}"/>
     <hyperlink ref="G11" r:id="rId7" location="reference-index" display="https://docs.python.org/3/reference/index.html#reference-index" xr:uid="{E1E283EA-7D9F-4134-91CD-45B539F1DABA}"/>
     <hyperlink ref="G12" r:id="rId8" display="https://docs.python.org/3/library/" xr:uid="{358221D7-1D16-4026-A041-393E9427BCB8}"/>
+    <hyperlink ref="G16" r:id="rId9" location="reader-comments" xr:uid="{5D8AFB6A-DB55-4E03-8161-2E5EC88E4340}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
starting to test ftau plus rigidbody
</commit_message>
<xml_diff>
--- a/mgt/Tasks.xlsx
+++ b/mgt/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E8A579-99F5-4941-938F-CE47005E26EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3184598A-DD92-40AD-87DD-84D95E4B86A1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,6 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>Python Tutorial/Course</t>
   </si>
@@ -124,13 +125,22 @@
     <t xml:space="preserve">read all again about first order systems </t>
   </si>
   <si>
-    <t xml:space="preserve">almost done, consider adding a motor FOS step response, and to add configurable noise </t>
-  </si>
-  <si>
     <t>https://realpython.com/python-matplotlib-guide/#reader-comments</t>
   </si>
   <si>
     <t>Create Quad model for forces and torques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to add x configuration </t>
+  </si>
+  <si>
+    <t xml:space="preserve">consider adding some dynamic response for the motors later when you find some docs for it </t>
+  </si>
+  <si>
+    <t>CAT</t>
+  </si>
+  <si>
+    <t>to add wind to the whole setup</t>
   </si>
 </sst>
 </file>
@@ -472,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,12 +494,13 @@
     <col min="2" max="2" width="41.44140625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="26.44140625" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" customWidth="1"/>
-    <col min="7" max="7" width="83.33203125" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" customWidth="1"/>
+    <col min="8" max="8" width="83.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
@@ -500,16 +511,19 @@
         <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -520,124 +534,130 @@
         <v>43634</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C3" s="2">
         <v>43635</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
       <c r="D4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="2">
-        <v>43635</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="E4" s="1"/>
+      <c r="F4" s="2">
+        <v>43635</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C7" s="2"/>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C8" s="2"/>
-      <c r="E8" s="2">
-        <v>43635</v>
-      </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="4" t="s">
+      <c r="F8" s="2">
+        <v>43635</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C9" s="2"/>
-      <c r="E9" s="2">
-        <v>43635</v>
-      </c>
-      <c r="F9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="4" t="s">
+      <c r="F9" s="2">
+        <v>43635</v>
+      </c>
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C10" s="2">
         <v>43635</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F10" t="s">
+      <c r="E10" s="1"/>
+      <c r="G10" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C11" s="2"/>
       <c r="D11" s="1"/>
-      <c r="G11" s="4" t="s">
+      <c r="E11" s="1"/>
+      <c r="H11" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C12" s="2"/>
       <c r="D12" s="1"/>
-      <c r="G12" s="4" t="s">
+      <c r="E12" s="1"/>
+      <c r="H12" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C13" s="2">
         <v>43636</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E13" s="1"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C14" s="2"/>
       <c r="D14" s="1"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E14" s="1"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -647,23 +667,23 @@
       <c r="C15" s="2">
         <v>43634</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C16" s="2">
         <v>43638</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C17" s="2"/>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3</v>
       </c>
@@ -673,14 +693,14 @@
       <c r="C18" s="2">
         <v>43634</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F18" s="2">
         <v>43636</v>
       </c>
-      <c r="F18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4</v>
       </c>
@@ -690,34 +710,34 @@
       <c r="C19" s="2">
         <v>43634</v>
       </c>
-      <c r="E19" s="2">
-        <v>43635</v>
-      </c>
-      <c r="F19" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="1" t="s">
+      <c r="F19" s="2">
+        <v>43635</v>
+      </c>
+      <c r="G19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="2">
         <v>43635</v>
       </c>
-      <c r="F20" t="s">
-        <v>10</v>
-      </c>
       <c r="G20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="H20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>6</v>
       </c>
@@ -727,14 +747,14 @@
       <c r="C21" s="2">
         <v>43635</v>
       </c>
-      <c r="E21" s="2">
-        <v>43635</v>
-      </c>
-      <c r="F21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F21" s="2">
+        <v>43635</v>
+      </c>
+      <c r="G21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>7</v>
       </c>
@@ -744,14 +764,14 @@
       <c r="C22" s="2">
         <v>43635</v>
       </c>
-      <c r="F22" t="s">
-        <v>17</v>
-      </c>
       <c r="G22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>8</v>
       </c>
@@ -761,17 +781,17 @@
       <c r="C23" s="2">
         <v>43635</v>
       </c>
-      <c r="E23" s="2">
+      <c r="F23" s="2">
         <v>43636</v>
       </c>
-      <c r="F23" t="s">
-        <v>17</v>
-      </c>
       <c r="G23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>9</v>
       </c>
@@ -781,38 +801,66 @@
       <c r="C24" s="2">
         <v>43636</v>
       </c>
-      <c r="E24" s="2">
+      <c r="F24" s="2">
         <v>43636</v>
       </c>
-      <c r="F24" t="s">
-        <v>17</v>
-      </c>
       <c r="G24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="2">
         <v>43637</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="2">
+        <v>43638</v>
+      </c>
+      <c r="G26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>11</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="2">
+        <v>43638</v>
+      </c>
+      <c r="G27" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G4" r:id="rId1" xr:uid="{9F407E9B-9C8D-4E2F-929C-8FDE3A9211C3}"/>
-    <hyperlink ref="G5" r:id="rId2" display="https://www.python.org/dev/peps/pep-0008/" xr:uid="{2115ECD9-1B72-4573-A8FF-B47D4F0E7727}"/>
-    <hyperlink ref="G6" r:id="rId3" display="https://www.python.org/dev/peps/pep-0257/" xr:uid="{A47415FF-60E2-4A53-89B4-48CD862F7193}"/>
-    <hyperlink ref="G8" r:id="rId4" xr:uid="{B7594100-27EE-4D55-A587-61F5DDEE6559}"/>
-    <hyperlink ref="G9" r:id="rId5" xr:uid="{B1A7EC17-81A5-4153-9ED0-990BA81AB5A2}"/>
-    <hyperlink ref="G7" r:id="rId6" location="why-we-need-pep-8" xr:uid="{BABF3B79-FEBC-4757-A901-5F528B5760A1}"/>
-    <hyperlink ref="G11" r:id="rId7" location="reference-index" display="https://docs.python.org/3/reference/index.html#reference-index" xr:uid="{E1E283EA-7D9F-4134-91CD-45B539F1DABA}"/>
-    <hyperlink ref="G12" r:id="rId8" display="https://docs.python.org/3/library/" xr:uid="{358221D7-1D16-4026-A041-393E9427BCB8}"/>
-    <hyperlink ref="G16" r:id="rId9" location="reader-comments" xr:uid="{5D8AFB6A-DB55-4E03-8161-2E5EC88E4340}"/>
+    <hyperlink ref="H4" r:id="rId1" xr:uid="{9F407E9B-9C8D-4E2F-929C-8FDE3A9211C3}"/>
+    <hyperlink ref="H5" r:id="rId2" display="https://www.python.org/dev/peps/pep-0008/" xr:uid="{2115ECD9-1B72-4573-A8FF-B47D4F0E7727}"/>
+    <hyperlink ref="H6" r:id="rId3" display="https://www.python.org/dev/peps/pep-0257/" xr:uid="{A47415FF-60E2-4A53-89B4-48CD862F7193}"/>
+    <hyperlink ref="H8" r:id="rId4" xr:uid="{B7594100-27EE-4D55-A587-61F5DDEE6559}"/>
+    <hyperlink ref="H9" r:id="rId5" xr:uid="{B1A7EC17-81A5-4153-9ED0-990BA81AB5A2}"/>
+    <hyperlink ref="H7" r:id="rId6" location="why-we-need-pep-8" xr:uid="{BABF3B79-FEBC-4757-A901-5F528B5760A1}"/>
+    <hyperlink ref="H11" r:id="rId7" location="reference-index" display="https://docs.python.org/3/reference/index.html#reference-index" xr:uid="{E1E283EA-7D9F-4134-91CD-45B539F1DABA}"/>
+    <hyperlink ref="H12" r:id="rId8" display="https://docs.python.org/3/library/" xr:uid="{358221D7-1D16-4026-A041-393E9427BCB8}"/>
+    <hyperlink ref="H16" r:id="rId9" location="reader-comments" xr:uid="{5D8AFB6A-DB55-4E03-8161-2E5EC88E4340}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>

</xml_diff>

<commit_message>
update in mgt folder. closing for today the 23rd
</commit_message>
<xml_diff>
--- a/mgt/Tasks.xlsx
+++ b/mgt/Tasks.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B41A86-92CF-405F-A8C3-F884FA0669CF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A3A115-F8D7-40D3-994F-E1C906C38D04}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="1" r:id="rId1"/>
     <sheet name="Reading" sheetId="2" r:id="rId2"/>
+    <sheet name="Course Materials" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
   <si>
     <t>TestCases for the RigidBody Class</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Status Date</t>
-  </si>
-  <si>
     <t>Ongoing</t>
   </si>
   <si>
@@ -139,6 +136,27 @@
   </si>
   <si>
     <t>Unit Tests for the quadftau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L001 Course introduction Video </t>
+  </si>
+  <si>
+    <t>Ideation</t>
+  </si>
+  <si>
+    <t>Closing date</t>
+  </si>
+  <si>
+    <t>Closing Date</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Bundle startup (slide templete, tools, folder structure)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L001 Course introduction Slides </t>
   </si>
 </sst>
 </file>
@@ -191,7 +209,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -199,6 +217,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -483,14 +503,14 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.88671875" customWidth="1"/>
     <col min="2" max="2" width="41.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" customWidth="1"/>
     <col min="5" max="5" width="11.77734375" customWidth="1"/>
     <col min="6" max="6" width="14.5546875" customWidth="1"/>
@@ -505,10 +525,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
@@ -532,13 +552,13 @@
         <v>43634</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" s="2">
         <v>43636</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -555,10 +575,10 @@
         <v>43635</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -566,22 +586,22 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2">
         <v>43635</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="2">
         <v>43637</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -589,19 +609,19 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2">
         <v>43638</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" s="2">
         <v>43638</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -609,19 +629,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2">
         <v>43635</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="2">
         <v>43635</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -629,19 +649,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2">
         <v>43635</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -649,22 +669,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2">
         <v>43635</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="2">
         <v>43636</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -672,22 +692,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="2">
         <v>43636</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="2">
         <v>43636</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -695,16 +715,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="2">
         <v>43638</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -712,16 +732,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="2">
         <v>43638</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -729,19 +749,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2">
         <v>43638</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13" s="2">
         <v>43639</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -772,57 +792,57 @@
       <c r="D2" s="1"/>
       <c r="E2" s="2"/>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" s="2"/>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -830,7 +850,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="G8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -838,24 +858,24 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="G9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="2">
         <v>43637</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -871,4 +891,124 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E82358F-0740-47A5-A144-DD54EE15A18A}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.44140625" customWidth="1"/>
+    <col min="2" max="2" width="44" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="6">
+        <v>43639</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="6">
+        <v>43639</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="6">
+        <v>43639</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="6">
+        <v>43639</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="2">
+        <v>43639</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
day's update of mgt folder
</commit_message>
<xml_diff>
--- a/mgt/Tasks.xlsx
+++ b/mgt/Tasks.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A3A115-F8D7-40D3-994F-E1C906C38D04}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D4D1D2-CEE9-46C1-BDCB-30A858AD6A1F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Code" sheetId="1" r:id="rId1"/>
-    <sheet name="Reading" sheetId="2" r:id="rId2"/>
-    <sheet name="Course Materials" sheetId="4" r:id="rId3"/>
+    <sheet name="Main Code" sheetId="1" r:id="rId1"/>
+    <sheet name="Visualization Code" sheetId="5" r:id="rId2"/>
+    <sheet name="Reading" sheetId="2" r:id="rId3"/>
+    <sheet name="Course Materials" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
   <si>
     <t>TestCases for the RigidBody Class</t>
   </si>
@@ -157,6 +158,33 @@
   </si>
   <si>
     <t xml:space="preserve">L001 Course introduction Slides </t>
+  </si>
+  <si>
+    <t>First tests with Panda3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Installed Panda3D in Anaconda. Modified the panda example  receive keys, and move the bear around. I also tested changing the HPR of the main actor </t>
+  </si>
+  <si>
+    <t>Idx</t>
+  </si>
+  <si>
+    <t>Attach camera to follow actor</t>
+  </si>
+  <si>
+    <t>Should be easy since now I have code setting the camera position</t>
+  </si>
+  <si>
+    <t>Explore envir and actor file formats</t>
+  </si>
+  <si>
+    <t>https://www.panda3d.org/manual/?title=Models_and_Actors</t>
+  </si>
+  <si>
+    <t>L002 Quadrotor Principles of Operaration Slides</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L003 Rigid Body Dynamics Slides </t>
   </si>
 </sst>
 </file>
@@ -209,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -219,6 +247,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -500,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,6 +549,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
@@ -538,130 +572,149 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C2" s="2"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>43634</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="2">
+        <v>43636</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C3" s="2">
         <v>43634</v>
       </c>
-      <c r="D3" t="s">
-        <v>33</v>
-      </c>
       <c r="E3" s="2">
-        <v>43636</v>
+        <v>43635</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
       </c>
       <c r="C4" s="2">
-        <v>43634</v>
+        <v>43635</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
       </c>
       <c r="E4" s="2">
-        <v>43635</v>
+        <v>43637</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>8</v>
+      <c r="G4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43638</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="2">
+        <v>43638</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2">
         <v>43635</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="2">
-        <v>43637</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="2">
-        <v>43638</v>
-      </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
       <c r="E6" s="2">
-        <v>43638</v>
+        <v>43635</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
+      <c r="B7" t="s">
+        <v>12</v>
       </c>
       <c r="C7" s="2">
         <v>43635</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="2">
-        <v>43635</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>12</v>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C8" s="2">
         <v>43635</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="E8" s="2">
+        <v>43636</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -669,13 +722,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2">
-        <v>43635</v>
+        <v>43636</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E9" s="2">
         <v>43636</v>
@@ -684,30 +737,24 @@
         <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C10" s="2">
-        <v>43636</v>
+        <v>43638</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="2">
-        <v>43636</v>
+        <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -715,7 +762,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2">
         <v>43638</v>
@@ -732,35 +779,18 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2">
         <v>43638</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="E12" s="2">
+        <v>43639</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="2">
-        <v>43638</v>
-      </c>
-      <c r="D13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="2">
-        <v>43639</v>
-      </c>
-      <c r="F13" t="s">
         <v>13</v>
       </c>
     </row>
@@ -771,6 +801,177 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A72FCC-3F51-403B-9627-94428C452F9B}">
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+    <col min="7" max="7" width="54.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="2">
+        <v>43640</v>
+      </c>
+      <c r="E2" s="2">
+        <v>43640</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="2">
+        <v>43640</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="2">
+        <v>43640</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G21" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G4" r:id="rId1" xr:uid="{EA196E6B-915D-4E85-8B73-9377741A52E0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BFE1673-F95D-4B86-96F0-1569AFA74034}">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -893,12 +1094,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E82358F-0740-47A5-A144-DD54EE15A18A}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -978,10 +1179,32 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43640</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="2">
+        <v>43640</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>

</xml_diff>

<commit_message>
new tests with Panda3D
</commit_message>
<xml_diff>
--- a/mgt/Tasks.xlsx
+++ b/mgt/Tasks.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD3594D-FB27-41E5-8515-5FAE75B350C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AEEBA86-9E84-437F-A048-BB285A1606B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Code" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="77">
   <si>
     <t>TestCases for the RigidBody Class</t>
   </si>
@@ -118,9 +118,6 @@
     <t>made a file but did not commit, I am not using it anywhere in the project</t>
   </si>
   <si>
-    <t>to add x configuration (only have  + now)</t>
-  </si>
-  <si>
     <t>Component testing rigidbody plus qftau</t>
   </si>
   <si>
@@ -133,9 +130,6 @@
     <t>DEV MISC</t>
   </si>
   <si>
-    <t>r</t>
-  </si>
-  <si>
     <t>Unit Tests for the quadftau</t>
   </si>
   <si>
@@ -172,9 +166,6 @@
     <t>Attach camera to follow actor</t>
   </si>
   <si>
-    <t>Should be easy since now I have code setting the camera position</t>
-  </si>
-  <si>
     <t>Explore envir and actor file formats</t>
   </si>
   <si>
@@ -190,9 +181,6 @@
     <t xml:space="preserve">L004 Rigid Body Dynamics Slides </t>
   </si>
   <si>
-    <t xml:space="preserve">Ongoing </t>
-  </si>
-  <si>
     <t>L002+L003 Slides and transcript</t>
   </si>
   <si>
@@ -211,9 +199,6 @@
     <t>L001+L002+L003 video, with noise red, udemy upload</t>
   </si>
   <si>
-    <t>ToDO</t>
-  </si>
-  <si>
     <t>IMPROVEMENT:  the rotm with diag elements with -1/2 , and multiplication by 2 just once. should be faster</t>
   </si>
   <si>
@@ -229,10 +214,46 @@
     <t>Record video for lecture 005</t>
   </si>
   <si>
-    <t>Lecture L006 - Flight Dynamics slides</t>
-  </si>
-  <si>
     <t>Record video for lecture 004</t>
+  </si>
+  <si>
+    <t>Lecture L006  slides</t>
+  </si>
+  <si>
+    <t>Investsigate implementation of Runge kutta ( at least RK4 )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investigate topic accelerometer not placed exactly at the center of mass - MEMS board alignment </t>
+  </si>
+  <si>
+    <t>Not much faster. Why is q slower than rotm ? And less precise in the short run. But rotm we get weird determinant over time.</t>
+  </si>
+  <si>
+    <t>to add x configuration (only have + now)</t>
+  </si>
+  <si>
+    <t>INS alignment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lecture 007  video </t>
+  </si>
+  <si>
+    <t>Should be easy since now I have code setting the camera position +camera.lookAt(object) function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quadrotor model </t>
+  </si>
+  <si>
+    <t>Manged with two Blender  addons, one to read  Google SketchuP format, and one to export to egg format. And found a *.skp file for the Crazyflie.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">video correct Lecture 3, 5 and Lecture 6 </t>
+  </si>
+  <si>
+    <t>Textures and Motion/Actor for the quadrotor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heavy work </t>
   </si>
 </sst>
 </file>
@@ -579,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,7 +619,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
@@ -610,7 +631,7 @@
         <v>28</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
@@ -630,7 +651,7 @@
         <v>43634</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="2">
         <v>43636</v>
@@ -670,7 +691,7 @@
         <v>43635</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="2">
         <v>43637</v>
@@ -687,13 +708,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" s="2">
         <v>43638</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="2">
         <v>43638</v>
@@ -713,7 +734,7 @@
         <v>43635</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" s="2">
         <v>43635</v>
@@ -733,7 +754,7 @@
         <v>43635</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
@@ -753,7 +774,7 @@
         <v>43635</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="2">
         <v>43636</v>
@@ -776,7 +797,7 @@
         <v>43636</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="2">
         <v>43636</v>
@@ -793,16 +814,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="C10" s="2">
         <v>43638</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="E10" s="2">
+        <v>43652</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -816,10 +840,10 @@
         <v>43638</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -827,13 +851,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="2">
         <v>43638</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="2">
         <v>43639</v>
@@ -847,16 +871,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C13" s="2">
         <v>43641</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -864,13 +888,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C14" s="2">
         <v>43642</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E14" s="2">
         <v>43642</v>
@@ -884,13 +908,33 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C15" s="2">
         <v>43647</v>
       </c>
+      <c r="E15" s="2">
+        <v>43652</v>
+      </c>
       <c r="F15" t="s">
-        <v>62</v>
+        <v>13</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="2">
+        <v>43652</v>
+      </c>
+      <c r="F16" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -903,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A72FCC-3F51-403B-9627-94428C452F9B}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -920,7 +964,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
@@ -932,7 +976,7 @@
         <v>28</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
@@ -946,7 +990,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2">
         <v>43640</v>
@@ -958,7 +1002,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -966,16 +1010,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3" s="2">
         <v>43640</v>
       </c>
+      <c r="E3" s="2">
+        <v>43652</v>
+      </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -983,7 +1030,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C4" s="2">
         <v>43640</v>
@@ -992,16 +1039,42 @@
         <v>14</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="G6" s="1"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="2">
+        <v>43652</v>
+      </c>
+      <c r="F5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="2">
+        <v>43652</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
@@ -1072,19 +1145,44 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BFE1673-F95D-4B86-96F0-1569AFA74034}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="7" max="7" width="80.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" s="2"/>
+      <c r="A1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
@@ -1161,10 +1259,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
+    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1176,6 +1271,20 @@
       </c>
       <c r="G10" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="2">
+        <v>43652</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1197,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E82358F-0740-47A5-A144-DD54EE15A18A}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1206,21 +1315,22 @@
     <col min="1" max="1" width="4.44140625" customWidth="1"/>
     <col min="2" max="2" width="44" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1"/>
     <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
@@ -1231,7 +1341,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" s="6">
         <v>43639</v>
@@ -1249,7 +1359,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C3" s="6">
         <v>43639</v>
@@ -1267,7 +1377,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" s="2">
         <v>43639</v>
@@ -1285,7 +1395,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C5" s="2">
         <v>43640</v>
@@ -1302,7 +1412,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C6" s="2">
         <v>43640</v>
@@ -1311,7 +1421,7 @@
         <v>43648</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1319,13 +1429,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C7" s="2">
         <v>43644</v>
       </c>
       <c r="F7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1333,7 +1443,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C8" s="2"/>
       <c r="E8" s="2">
@@ -1348,7 +1458,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C9" s="2">
         <v>43645</v>
@@ -1357,7 +1467,7 @@
         <v>43648</v>
       </c>
       <c r="F9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1365,7 +1475,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C10" s="2">
         <v>43645</v>
@@ -1379,7 +1489,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C11" s="2">
         <v>43645</v>
@@ -1396,7 +1506,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C12" s="2">
         <v>43645</v>
@@ -1413,7 +1523,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C13" s="2">
         <v>43648</v>
@@ -1430,22 +1540,42 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C14" s="2">
         <v>43645</v>
       </c>
+      <c r="E14" s="2">
+        <v>43651</v>
+      </c>
       <c r="F14" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="1"/>
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="2">
+        <v>43652</v>
+      </c>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="1"/>
+      <c r="A16" s="5">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>

</xml_diff>

<commit_message>
changed rigid body to ve as state and the eq of motion
</commit_message>
<xml_diff>
--- a/mgt/Tasks.xlsx
+++ b/mgt/Tasks.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C7AC8A-CF71-4934-B83B-2F05714551FC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF3F488-675D-4A2C-86EF-FFB0BB5C8F4B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Code" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="79">
   <si>
     <t>TestCases for the RigidBody Class</t>
   </si>
@@ -263,6 +263,9 @@
   </si>
   <si>
     <t xml:space="preserve">Lecture 008 slides </t>
+  </si>
+  <si>
+    <t>Investigate better step responses for both cross and plus configuration</t>
   </si>
 </sst>
 </file>
@@ -609,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -944,6 +947,20 @@
       </c>
       <c r="F16" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="2">
+        <v>43654</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1330,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E82358F-0740-47A5-A144-DD54EE15A18A}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F18" sqref="A18:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1618,9 +1635,6 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="1"/>
-    </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
     </row>

</xml_diff>

<commit_message>
added PID control for flight stabilization, first version raw
</commit_message>
<xml_diff>
--- a/mgt/Tasks.xlsx
+++ b/mgt/Tasks.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A8B069-367A-400A-8DDA-46D058480164}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C75771-9B0F-4DEE-AF70-6BB94B047104}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Code" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="80">
   <si>
     <t>TestCases for the RigidBody Class</t>
   </si>
@@ -266,6 +266,9 @@
   </si>
   <si>
     <t xml:space="preserve">Lecture 008 slides &amp; video </t>
+  </si>
+  <si>
+    <t>17 Lie group integration techniques for quaternions</t>
   </si>
 </sst>
 </file>
@@ -612,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -960,6 +963,17 @@
         <v>43654</v>
       </c>
       <c r="F17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="2">
+        <v>43654</v>
+      </c>
+      <c r="F18" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1347,8 +1361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E82358F-0740-47A5-A144-DD54EE15A18A}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update mainly in the att stab
</commit_message>
<xml_diff>
--- a/mgt/Tasks.xlsx
+++ b/mgt/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C75771-9B0F-4DEE-AF70-6BB94B047104}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A534C4-F5AD-421A-A075-74300690DA26}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="84">
   <si>
     <t>TestCases for the RigidBody Class</t>
   </si>
@@ -269,6 +269,18 @@
   </si>
   <si>
     <t>17 Lie group integration techniques for quaternions</t>
+  </si>
+  <si>
+    <t>Correct euler angles so we do not have a jump, not good  for my att stab (yaw case)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make propellers move </t>
+  </si>
+  <si>
+    <t>Attitude stabilization with PID</t>
+  </si>
+  <si>
+    <t>IMPROVEMENT</t>
   </si>
 </sst>
 </file>
@@ -615,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,7 +638,7 @@
     <col min="1" max="1" width="2.88671875" customWidth="1"/>
     <col min="2" max="2" width="41.44140625" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
     <col min="5" max="5" width="11.77734375" customWidth="1"/>
     <col min="6" max="6" width="14.5546875" customWidth="1"/>
     <col min="7" max="7" width="83.33203125" customWidth="1"/>
@@ -928,6 +940,9 @@
       <c r="C15" s="2">
         <v>43647</v>
       </c>
+      <c r="D15" t="s">
+        <v>83</v>
+      </c>
       <c r="E15" s="2">
         <v>43652</v>
       </c>
@@ -948,6 +963,9 @@
       <c r="C16" s="2">
         <v>43652</v>
       </c>
+      <c r="D16" t="s">
+        <v>83</v>
+      </c>
       <c r="F16" t="s">
         <v>55</v>
       </c>
@@ -973,8 +991,48 @@
       <c r="C18" s="2">
         <v>43654</v>
       </c>
+      <c r="D18" t="s">
+        <v>83</v>
+      </c>
       <c r="F18" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="2">
+        <v>43655</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="2">
+        <v>43655</v>
+      </c>
+      <c r="D20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="2">
+        <v>43656</v>
+      </c>
+      <c r="F20" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -988,7 +1046,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1130,7 +1188,9 @@
       <c r="F7" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">

</xml_diff>

<commit_message>
added control simulation. Position control is not finished. We need better PIDs.
</commit_message>
<xml_diff>
--- a/mgt/Tasks.xlsx
+++ b/mgt/Tasks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A534C4-F5AD-421A-A075-74300690DA26}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5EB240-7DA9-46B3-81F9-614241DCF0C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,6 +14,7 @@
     <sheet name="Course Materials" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="87">
   <si>
     <t>TestCases for the RigidBody Class</t>
   </si>
@@ -281,6 +282,15 @@
   </si>
   <si>
     <t>IMPROVEMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lecture 009: code package, slides and video </t>
+  </si>
+  <si>
+    <t>Simulation is faster than realt-time, which is good, but how to make it real time though</t>
+  </si>
+  <si>
+    <t>IMRPOVMENT</t>
   </si>
 </sst>
 </file>
@@ -627,24 +637,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" customWidth="1"/>
-    <col min="2" max="2" width="41.44140625" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" customWidth="1"/>
-    <col min="7" max="7" width="83.33203125" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="83.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>45</v>
       </c>
@@ -667,7 +677,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -687,7 +697,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -707,7 +717,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -730,7 +740,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -750,7 +760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -770,7 +780,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -790,7 +800,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -813,7 +823,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -836,7 +846,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -856,7 +866,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -873,7 +883,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -893,7 +903,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -910,7 +920,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -930,7 +940,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -953,7 +963,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -970,7 +980,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -984,7 +994,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -998,7 +1008,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1015,7 +1025,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1033,6 +1043,20 @@
       </c>
       <c r="F20" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="2">
+        <v>43660</v>
+      </c>
+      <c r="D21" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1049,18 +1073,18 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="36.21875" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" customWidth="1"/>
-    <col min="7" max="7" width="54.77734375" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="54.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>45</v>
       </c>
@@ -1083,7 +1107,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1103,7 +1127,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1123,7 +1147,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1140,7 +1164,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1157,7 +1181,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1175,7 +1199,7 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1192,61 +1216,61 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G21" s="1"/>
     </row>
   </sheetData>
@@ -1266,17 +1290,17 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
-    <col min="7" max="7" width="80.21875" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="80.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>45</v>
       </c>
@@ -1299,7 +1323,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1311,7 +1335,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="F3" t="s">
         <v>6</v>
@@ -1320,7 +1344,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="F4" t="s">
         <v>14</v>
@@ -1329,7 +1353,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="F5" t="s">
         <v>14</v>
@@ -1338,7 +1362,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" t="s">
@@ -1348,7 +1372,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" t="s">
@@ -1358,7 +1382,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1366,7 +1390,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1374,7 +1398,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1388,7 +1412,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>69</v>
       </c>
@@ -1422,20 +1446,20 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="2" width="44" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3" t="s">
@@ -1451,7 +1475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1469,7 +1493,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1487,7 +1511,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1505,7 +1529,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1522,7 +1546,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1539,7 +1563,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1553,7 +1577,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1568,7 +1592,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1585,7 +1609,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1599,7 +1623,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1616,7 +1640,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1633,7 +1657,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1650,7 +1674,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1667,7 +1691,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1684,7 +1708,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1701,7 +1725,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1712,40 +1736,54 @@
         <v>43653</v>
       </c>
       <c r="F17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="2">
+        <v>43658</v>
+      </c>
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
     </row>
   </sheetData>

</xml_diff>